<commit_message>
Ajout de la fonction secondaire
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_compas.xlsx
+++ b/fichiers/conf/modele_compas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266D027A-488A-4531-86A8-3A9D19D2AB45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FCF05C-1E21-4941-A15F-E759226F7520}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="690" windowWidth="24870" windowHeight="13320" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="330" yWindow="1785" windowWidth="24870" windowHeight="13320" tabRatio="591" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Compas" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Aide" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Compas!$A$1:$Q$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Compas!$A$1:$R$2</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -42,7 +42,7 @@
     <author>Sébastien</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{E61AC8E6-5369-486E-BB2A-CFC3F3BBFC62}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{E61AC8E6-5369-486E-BB2A-CFC3F3BBFC62}">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{BD73F079-BD47-4A9B-9DB9-888F403257F2}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{BD73F079-BD47-4A9B-9DB9-888F403257F2}">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{D7CCADB1-4D8A-4BC8-905C-D1BA438E77F1}">
       <text>
         <r>
           <rPr>
@@ -114,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{E9756D3C-D426-47A5-A95D-19409772C521}">
       <text>
         <r>
           <rPr>
@@ -138,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C19C0D7F-4226-4736-BA35-E6E08EBBAC7A}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{AB0FF933-2837-4C7D-A183-D59581906014}">
       <text>
         <r>
           <rPr>
@@ -186,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{783213B1-12E4-4FD7-BD87-ED5859C4959C}">
       <text>
         <r>
           <rPr>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>${chef.nom}</t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>${chef.formation.fc2.datefin}</t>
+  </si>
+  <si>
+    <t>Fonction secondaire</t>
+  </si>
+  <si>
+    <t>${chef.fonctionsecondairecomplet}</t>
   </si>
 </sst>
 </file>
@@ -523,7 +529,107 @@
     <cellStyle name="Filler1" xfId="1" xr:uid="{23D6D387-F5AE-44CD-BDE2-B1DB25CA5EB4}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF007E39"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -958,7 +1064,7 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
@@ -975,19 +1081,19 @@
     <col min="4" max="4" width="57.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="11.42578125" style="15" customWidth="1"/>
-    <col min="14" max="14" width="4" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" style="15" customWidth="1"/>
+    <col min="15" max="15" width="4" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="11" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1009,38 +1115,41 @@
       <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -1062,68 +1171,103 @@
       <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="15" t="s">
+      <c r="H2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="2"/>
+      <c r="M2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="2"/>
+      <c r="P2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q2" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
-  <conditionalFormatting sqref="P2:Q65535">
-    <cfRule type="cellIs" dxfId="10" priority="24" stopIfTrue="1" operator="equal">
+  <autoFilter ref="A1:R2" xr:uid="{D6BF73C0-3DFA-4EF7-83FF-A6F179361B6B}"/>
+  <conditionalFormatting sqref="Q2:R65535">
+    <cfRule type="cellIs" dxfId="20" priority="34" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65535">
+    <cfRule type="beginsWith" dxfId="19" priority="11" stopIfTrue="1" operator="beginsWith" text="14">
+      <formula>LEFT(G2,LEN("14"))="14"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="18" priority="44" stopIfTrue="1" operator="beginsWith" text="6">
+      <formula>LEFT(G2,LEN("6"))="6"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="17" priority="45" stopIfTrue="1" operator="beginsWith" text="5">
+      <formula>LEFT(G2,LEN("5"))="5"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="46" stopIfTrue="1" operator="beginsWith" text="4">
+      <formula>LEFT(G2,LEN("4"))="4"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="15" priority="81" stopIfTrue="1" operator="beginsWith" text="24">
+      <formula>LEFT(G2,LEN("24"))="24"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="14" priority="82" stopIfTrue="1" operator="beginsWith" text="27">
+      <formula>LEFT(G2,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="13" priority="83" stopIfTrue="1" operator="beginsWith" text="3">
+      <formula>LEFT(G2,LEN("3"))="3"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="12" priority="84" stopIfTrue="1" operator="beginsWith" text="23">
+      <formula>LEFT(G2,LEN("23"))="23"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="11" priority="85" stopIfTrue="1" operator="beginsWith" text="22">
+      <formula>LEFT(G2,LEN("22"))="22"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="10" priority="86" stopIfTrue="1" operator="beginsWith" text="21">
+      <formula>LEFT(G2,LEN("21"))="21"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H65535">
     <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="14">
-      <formula>LEFT(G2,LEN("14"))="14"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="34" stopIfTrue="1" operator="beginsWith" text="6">
-      <formula>LEFT(G2,LEN("6"))="6"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="35" stopIfTrue="1" operator="beginsWith" text="5">
-      <formula>LEFT(G2,LEN("5"))="5"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="36" stopIfTrue="1" operator="beginsWith" text="4">
-      <formula>LEFT(G2,LEN("4"))="4"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="71" stopIfTrue="1" operator="beginsWith" text="24">
-      <formula>LEFT(G2,LEN("24"))="24"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="72" stopIfTrue="1" operator="beginsWith" text="27">
-      <formula>LEFT(G2,LEN("27"))="27"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="73" stopIfTrue="1" operator="beginsWith" text="3">
-      <formula>LEFT(G2,LEN("3"))="3"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="74" stopIfTrue="1" operator="beginsWith" text="23">
-      <formula>LEFT(G2,LEN("23"))="23"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="75" stopIfTrue="1" operator="beginsWith" text="22">
-      <formula>LEFT(G2,LEN("22"))="22"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="76" stopIfTrue="1" operator="beginsWith" text="21">
-      <formula>LEFT(G2,LEN("21"))="21"</formula>
+      <formula>LEFT(H2,LEN("14"))="14"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="6">
+      <formula>LEFT(H2,LEN("6"))="6"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="7" priority="3" stopIfTrue="1" operator="beginsWith" text="5">
+      <formula>LEFT(H2,LEN("5"))="5"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="6" priority="4" stopIfTrue="1" operator="beginsWith" text="4">
+      <formula>LEFT(H2,LEN("4"))="4"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="5" stopIfTrue="1" operator="beginsWith" text="24">
+      <formula>LEFT(H2,LEN("24"))="24"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="6" stopIfTrue="1" operator="beginsWith" text="27">
+      <formula>LEFT(H2,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="beginsWith" text="3">
+      <formula>LEFT(H2,LEN("3"))="3"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="beginsWith" text="23">
+      <formula>LEFT(H2,LEN("23"))="23"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="beginsWith" text="22">
+      <formula>LEFT(H2,LEN("22"))="22"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="beginsWith" text="21">
+      <formula>LEFT(H2,LEN("21"))="21"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>